<commit_message>
Extend draft range to 14 meters with corresponding displacement data
Co-authored-by: tanmegan05-droid <253447754+tanmegan05-droid@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/MV_Del_Monte_Ship_Data.xlsx
+++ b/data/MV_Del_Monte_Ship_Data.xlsx
@@ -583,7 +583,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -705,6 +705,102 @@
       </c>
       <c r="B14" t="n">
         <v>9140</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="B15" t="n">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>9</v>
+      </c>
+      <c r="B16" t="n">
+        <v>10480</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="B17" t="n">
+        <v>11180</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>10</v>
+      </c>
+      <c r="B18" t="n">
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="B19" t="n">
+        <v>12640</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>11</v>
+      </c>
+      <c r="B20" t="n">
+        <v>13400</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="B21" t="n">
+        <v>14180</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>12</v>
+      </c>
+      <c r="B22" t="n">
+        <v>14980</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="B23" t="n">
+        <v>15800</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>13</v>
+      </c>
+      <c r="B24" t="n">
+        <v>16640</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="B25" t="n">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>14</v>
+      </c>
+      <c r="B26" t="n">
+        <v>18380</v>
       </c>
     </row>
   </sheetData>
@@ -718,7 +814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1206,6 +1302,804 @@
         <v>4.88</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>8500</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4</v>
+      </c>
+      <c r="I13" t="n">
+        <v>4.37</v>
+      </c>
+      <c r="J13" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="K13" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="L13" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>9000</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="F14" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="H14" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="J14" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="K14" t="n">
+        <v>5.17</v>
+      </c>
+      <c r="L14" t="n">
+        <v>5.32</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>9500</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="H15" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="I15" t="n">
+        <v>4.71</v>
+      </c>
+      <c r="J15" t="n">
+        <v>5.07</v>
+      </c>
+      <c r="K15" t="n">
+        <v>5.38</v>
+      </c>
+      <c r="L15" t="n">
+        <v>5.54</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="H16" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="I16" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="K16" t="n">
+        <v>5.59</v>
+      </c>
+      <c r="L16" t="n">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>10500</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="G17" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="I17" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="J17" t="n">
+        <v>5.45</v>
+      </c>
+      <c r="K17" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="L17" t="n">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>11000</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="F18" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="G18" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="H18" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="I18" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="J18" t="n">
+        <v>5.64</v>
+      </c>
+      <c r="K18" t="n">
+        <v>6.01</v>
+      </c>
+      <c r="L18" t="n">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>11500</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="F19" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="G19" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="H19" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="I19" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="J19" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="K19" t="n">
+        <v>6.22</v>
+      </c>
+      <c r="L19" t="n">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>12000</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3.88</v>
+      </c>
+      <c r="G20" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="H20" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I20" t="n">
+        <v>5.56</v>
+      </c>
+      <c r="J20" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="K20" t="n">
+        <v>6.43</v>
+      </c>
+      <c r="L20" t="n">
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>12500</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="G21" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="H21" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="I21" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="J21" t="n">
+        <v>6.21</v>
+      </c>
+      <c r="K21" t="n">
+        <v>6.64</v>
+      </c>
+      <c r="L21" t="n">
+        <v>6.86</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>13000</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="F22" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="H22" t="n">
+        <v>5.35</v>
+      </c>
+      <c r="I22" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="J22" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="K22" t="n">
+        <v>6.85</v>
+      </c>
+      <c r="L22" t="n">
+        <v>7.08</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>13500</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2.72</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="F23" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="G23" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="H23" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="I23" t="n">
+        <v>6.07</v>
+      </c>
+      <c r="J23" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="K23" t="n">
+        <v>7.06</v>
+      </c>
+      <c r="L23" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>14000</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="F24" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="G24" t="n">
+        <v>5.01</v>
+      </c>
+      <c r="H24" t="n">
+        <v>5.65</v>
+      </c>
+      <c r="I24" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="J24" t="n">
+        <v>6.78</v>
+      </c>
+      <c r="K24" t="n">
+        <v>7.27</v>
+      </c>
+      <c r="L24" t="n">
+        <v>7.52</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>14500</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="F25" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="G25" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="H25" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="I25" t="n">
+        <v>6.41</v>
+      </c>
+      <c r="J25" t="n">
+        <v>6.97</v>
+      </c>
+      <c r="K25" t="n">
+        <v>7.48</v>
+      </c>
+      <c r="L25" t="n">
+        <v>7.74</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>15000</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5.27</v>
+      </c>
+      <c r="H26" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="I26" t="n">
+        <v>6.58</v>
+      </c>
+      <c r="J26" t="n">
+        <v>7.16</v>
+      </c>
+      <c r="K26" t="n">
+        <v>7.69</v>
+      </c>
+      <c r="L26" t="n">
+        <v>7.96</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>15500</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="D27" t="n">
+        <v>3</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="F27" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="H27" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="J27" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="K27" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="L27" t="n">
+        <v>8.18</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>16000</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="D28" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="F28" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5.53</v>
+      </c>
+      <c r="H28" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I28" t="n">
+        <v>6.92</v>
+      </c>
+      <c r="J28" t="n">
+        <v>7.54</v>
+      </c>
+      <c r="K28" t="n">
+        <v>8.109999999999999</v>
+      </c>
+      <c r="L28" t="n">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>16500</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="E29" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="F29" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="G29" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="H29" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="I29" t="n">
+        <v>7.09</v>
+      </c>
+      <c r="J29" t="n">
+        <v>7.73</v>
+      </c>
+      <c r="K29" t="n">
+        <v>8.32</v>
+      </c>
+      <c r="L29" t="n">
+        <v>8.619999999999999</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>17000</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="C30" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="E30" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="F30" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="G30" t="n">
+        <v>5.79</v>
+      </c>
+      <c r="H30" t="n">
+        <v>6.55</v>
+      </c>
+      <c r="I30" t="n">
+        <v>7.26</v>
+      </c>
+      <c r="J30" t="n">
+        <v>7.92</v>
+      </c>
+      <c r="K30" t="n">
+        <v>8.529999999999999</v>
+      </c>
+      <c r="L30" t="n">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>17500</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="C31" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D31" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="E31" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="F31" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="H31" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="I31" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="J31" t="n">
+        <v>8.109999999999999</v>
+      </c>
+      <c r="K31" t="n">
+        <v>8.74</v>
+      </c>
+      <c r="L31" t="n">
+        <v>9.06</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>18000</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="E32" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="F32" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="G32" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="H32" t="n">
+        <v>6.85</v>
+      </c>
+      <c r="I32" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="J32" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="K32" t="n">
+        <v>8.949999999999999</v>
+      </c>
+      <c r="L32" t="n">
+        <v>9.279999999999999</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>18500</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D33" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4.39</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="G33" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="H33" t="n">
+        <v>7</v>
+      </c>
+      <c r="I33" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="J33" t="n">
+        <v>8.49</v>
+      </c>
+      <c r="K33" t="n">
+        <v>9.16</v>
+      </c>
+      <c r="L33" t="n">
+        <v>9.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct displacement values - 12m draft now shows 70,667 tonnes
Co-authored-by: tanmegan05-droid <253447754+tanmegan05-droid@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/MV_Del_Monte_Ship_Data.xlsx
+++ b/data/MV_Del_Monte_Ship_Data.xlsx
@@ -608,7 +608,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>2800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="3">
@@ -616,7 +616,7 @@
         <v>2.5</v>
       </c>
       <c r="B3" t="n">
-        <v>3200</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="4">
@@ -624,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3650</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="5">
@@ -632,7 +632,7 @@
         <v>3.5</v>
       </c>
       <c r="B5" t="n">
-        <v>4100</v>
+        <v>3247</v>
       </c>
     </row>
     <row r="6">
@@ -640,7 +640,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>4580</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="7">
@@ -648,7 +648,7 @@
         <v>4.5</v>
       </c>
       <c r="B7" t="n">
-        <v>5080</v>
+        <v>6085</v>
       </c>
     </row>
     <row r="8">
@@ -656,7 +656,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="n">
-        <v>5600</v>
+        <v>7919</v>
       </c>
     </row>
     <row r="9">
@@ -664,7 +664,7 @@
         <v>5.5</v>
       </c>
       <c r="B9" t="n">
-        <v>6140</v>
+        <v>10050</v>
       </c>
     </row>
     <row r="10">
@@ -672,7 +672,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="n">
-        <v>6700</v>
+        <v>12492</v>
       </c>
     </row>
     <row r="11">
@@ -680,7 +680,7 @@
         <v>6.5</v>
       </c>
       <c r="B11" t="n">
-        <v>7280</v>
+        <v>15260</v>
       </c>
     </row>
     <row r="12">
@@ -688,7 +688,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="n">
-        <v>7880</v>
+        <v>18366</v>
       </c>
     </row>
     <row r="13">
@@ -696,7 +696,7 @@
         <v>7.5</v>
       </c>
       <c r="B13" t="n">
-        <v>8500</v>
+        <v>21823</v>
       </c>
     </row>
     <row r="14">
@@ -704,7 +704,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="n">
-        <v>9140</v>
+        <v>25644</v>
       </c>
     </row>
     <row r="15">
@@ -712,7 +712,7 @@
         <v>8.5</v>
       </c>
       <c r="B15" t="n">
-        <v>9800</v>
+        <v>29841</v>
       </c>
     </row>
     <row r="16">
@@ -720,7 +720,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="n">
-        <v>10480</v>
+        <v>34425</v>
       </c>
     </row>
     <row r="17">
@@ -728,7 +728,7 @@
         <v>9.5</v>
       </c>
       <c r="B17" t="n">
-        <v>11180</v>
+        <v>39407</v>
       </c>
     </row>
     <row r="18">
@@ -736,7 +736,7 @@
         <v>10</v>
       </c>
       <c r="B18" t="n">
-        <v>11900</v>
+        <v>44799</v>
       </c>
     </row>
     <row r="19">
@@ -744,7 +744,7 @@
         <v>10.5</v>
       </c>
       <c r="B19" t="n">
-        <v>12640</v>
+        <v>50610</v>
       </c>
     </row>
     <row r="20">
@@ -752,7 +752,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="n">
-        <v>13400</v>
+        <v>56852</v>
       </c>
     </row>
     <row r="21">
@@ -760,7 +760,7 @@
         <v>11.5</v>
       </c>
       <c r="B21" t="n">
-        <v>14180</v>
+        <v>63534</v>
       </c>
     </row>
     <row r="22">
@@ -768,7 +768,7 @@
         <v>12</v>
       </c>
       <c r="B22" t="n">
-        <v>14980</v>
+        <v>70667</v>
       </c>
     </row>
     <row r="23">
@@ -776,7 +776,7 @@
         <v>12.5</v>
       </c>
       <c r="B23" t="n">
-        <v>15800</v>
+        <v>78260</v>
       </c>
     </row>
     <row r="24">
@@ -784,7 +784,7 @@
         <v>13</v>
       </c>
       <c r="B24" t="n">
-        <v>16640</v>
+        <v>86322</v>
       </c>
     </row>
     <row r="25">
@@ -792,7 +792,7 @@
         <v>13.5</v>
       </c>
       <c r="B25" t="n">
-        <v>17500</v>
+        <v>94863</v>
       </c>
     </row>
     <row r="26">
@@ -800,7 +800,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="n">
-        <v>18380</v>
+        <v>103892</v>
       </c>
     </row>
   </sheetData>
@@ -814,7 +814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -886,1218 +886,1522 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="B2" t="n">
-        <v>0.45</v>
+        <v>0.51</v>
       </c>
       <c r="C2" t="n">
-        <v>0.85</v>
+        <v>0.98</v>
       </c>
       <c r="D2" t="n">
-        <v>1.25</v>
+        <v>1.58</v>
       </c>
       <c r="E2" t="n">
-        <v>1.6</v>
+        <v>2.3</v>
       </c>
       <c r="F2" t="n">
-        <v>1.9</v>
+        <v>3.14</v>
       </c>
       <c r="G2" t="n">
-        <v>2.15</v>
+        <v>4.08</v>
       </c>
       <c r="H2" t="n">
-        <v>2.35</v>
+        <v>5.11</v>
       </c>
       <c r="I2" t="n">
-        <v>2.5</v>
+        <v>6.22</v>
       </c>
       <c r="J2" t="n">
-        <v>2.6</v>
+        <v>7.38</v>
       </c>
       <c r="K2" t="n">
-        <v>2.65</v>
+        <v>8.57</v>
       </c>
       <c r="L2" t="n">
-        <v>2.68</v>
+        <v>9.789999999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3500</v>
+        <v>3795</v>
       </c>
       <c r="B3" t="n">
-        <v>0.48</v>
+        <v>1.13</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9</v>
+        <v>2.17</v>
       </c>
       <c r="D3" t="n">
-        <v>1.32</v>
+        <v>3.51</v>
       </c>
       <c r="E3" t="n">
-        <v>1.69</v>
+        <v>5.12</v>
       </c>
       <c r="F3" t="n">
-        <v>2.01</v>
+        <v>6.99</v>
       </c>
       <c r="G3" t="n">
-        <v>2.28</v>
+        <v>9.09</v>
       </c>
       <c r="H3" t="n">
-        <v>2.5</v>
+        <v>11.38</v>
       </c>
       <c r="I3" t="n">
-        <v>2.67</v>
+        <v>13.84</v>
       </c>
       <c r="J3" t="n">
-        <v>2.79</v>
+        <v>16.42</v>
       </c>
       <c r="K3" t="n">
-        <v>2.86</v>
+        <v>19.08</v>
       </c>
       <c r="L3" t="n">
-        <v>2.9</v>
+        <v>21.79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4000</v>
+        <v>6590</v>
       </c>
       <c r="B4" t="n">
-        <v>0.51</v>
+        <v>1.58</v>
       </c>
       <c r="C4" t="n">
-        <v>0.95</v>
+        <v>3.02</v>
       </c>
       <c r="D4" t="n">
-        <v>1.39</v>
+        <v>4.88</v>
       </c>
       <c r="E4" t="n">
-        <v>1.78</v>
+        <v>7.13</v>
       </c>
       <c r="F4" t="n">
-        <v>2.12</v>
+        <v>9.73</v>
       </c>
       <c r="G4" t="n">
-        <v>2.41</v>
+        <v>12.65</v>
       </c>
       <c r="H4" t="n">
-        <v>2.65</v>
+        <v>15.85</v>
       </c>
       <c r="I4" t="n">
-        <v>2.84</v>
+        <v>19.27</v>
       </c>
       <c r="J4" t="n">
-        <v>2.98</v>
+        <v>22.86</v>
       </c>
       <c r="K4" t="n">
-        <v>3.07</v>
+        <v>26.58</v>
       </c>
       <c r="L4" t="n">
-        <v>3.12</v>
+        <v>30.34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4500</v>
+        <v>9385</v>
       </c>
       <c r="B5" t="n">
-        <v>0.54</v>
+        <v>1.95</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>3.74</v>
       </c>
       <c r="D5" t="n">
-        <v>1.46</v>
+        <v>6.04</v>
       </c>
       <c r="E5" t="n">
-        <v>1.87</v>
+        <v>8.81</v>
       </c>
       <c r="F5" t="n">
-        <v>2.23</v>
+        <v>12.03</v>
       </c>
       <c r="G5" t="n">
-        <v>2.54</v>
+        <v>15.64</v>
       </c>
       <c r="H5" t="n">
-        <v>2.8</v>
+        <v>19.59</v>
       </c>
       <c r="I5" t="n">
-        <v>3.01</v>
+        <v>23.82</v>
       </c>
       <c r="J5" t="n">
-        <v>3.17</v>
+        <v>28.27</v>
       </c>
       <c r="K5" t="n">
-        <v>3.28</v>
+        <v>32.86</v>
       </c>
       <c r="L5" t="n">
-        <v>3.34</v>
+        <v>37.51</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5000</v>
+        <v>12179</v>
       </c>
       <c r="B6" t="n">
-        <v>0.57</v>
+        <v>2.28</v>
       </c>
       <c r="C6" t="n">
-        <v>1.05</v>
+        <v>4.37</v>
       </c>
       <c r="D6" t="n">
-        <v>1.53</v>
+        <v>7.06</v>
       </c>
       <c r="E6" t="n">
-        <v>1.96</v>
+        <v>10.31</v>
       </c>
       <c r="F6" t="n">
-        <v>2.34</v>
+        <v>14.07</v>
       </c>
       <c r="G6" t="n">
-        <v>2.67</v>
+        <v>18.29</v>
       </c>
       <c r="H6" t="n">
-        <v>2.95</v>
+        <v>22.91</v>
       </c>
       <c r="I6" t="n">
-        <v>3.18</v>
+        <v>27.86</v>
       </c>
       <c r="J6" t="n">
-        <v>3.36</v>
+        <v>33.05</v>
       </c>
       <c r="K6" t="n">
-        <v>3.49</v>
+        <v>38.42</v>
       </c>
       <c r="L6" t="n">
-        <v>3.56</v>
+        <v>43.87</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5500</v>
+        <v>14974</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6</v>
+        <v>2.58</v>
       </c>
       <c r="C7" t="n">
-        <v>1.1</v>
+        <v>4.95</v>
       </c>
       <c r="D7" t="n">
-        <v>1.6</v>
+        <v>7.99</v>
       </c>
       <c r="E7" t="n">
-        <v>2.05</v>
+        <v>11.67</v>
       </c>
       <c r="F7" t="n">
-        <v>2.45</v>
+        <v>15.93</v>
       </c>
       <c r="G7" t="n">
-        <v>2.8</v>
+        <v>20.71</v>
       </c>
       <c r="H7" t="n">
-        <v>3.1</v>
+        <v>25.93</v>
       </c>
       <c r="I7" t="n">
-        <v>3.35</v>
+        <v>31.53</v>
       </c>
       <c r="J7" t="n">
-        <v>3.55</v>
+        <v>37.41</v>
       </c>
       <c r="K7" t="n">
-        <v>3.7</v>
+        <v>43.49</v>
       </c>
       <c r="L7" t="n">
-        <v>3.78</v>
+        <v>49.65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6000</v>
+        <v>17769</v>
       </c>
       <c r="B8" t="n">
-        <v>0.63</v>
+        <v>2.86</v>
       </c>
       <c r="C8" t="n">
-        <v>1.15</v>
+        <v>5.48</v>
       </c>
       <c r="D8" t="n">
-        <v>1.67</v>
+        <v>8.85</v>
       </c>
       <c r="E8" t="n">
-        <v>2.14</v>
+        <v>12.93</v>
       </c>
       <c r="F8" t="n">
-        <v>2.56</v>
+        <v>17.65</v>
       </c>
       <c r="G8" t="n">
-        <v>2.93</v>
+        <v>22.95</v>
       </c>
       <c r="H8" t="n">
-        <v>3.25</v>
+        <v>28.74</v>
       </c>
       <c r="I8" t="n">
-        <v>3.52</v>
+        <v>34.94</v>
       </c>
       <c r="J8" t="n">
-        <v>3.74</v>
+        <v>41.46</v>
       </c>
       <c r="K8" t="n">
-        <v>3.91</v>
+        <v>48.19</v>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>55.02</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6500</v>
+        <v>20564</v>
       </c>
       <c r="B9" t="n">
-        <v>0.66</v>
+        <v>3.12</v>
       </c>
       <c r="C9" t="n">
-        <v>1.2</v>
+        <v>5.98</v>
       </c>
       <c r="D9" t="n">
-        <v>1.74</v>
+        <v>9.66</v>
       </c>
       <c r="E9" t="n">
-        <v>2.23</v>
+        <v>14.11</v>
       </c>
       <c r="F9" t="n">
-        <v>2.67</v>
+        <v>19.27</v>
       </c>
       <c r="G9" t="n">
-        <v>3.06</v>
+        <v>25.05</v>
       </c>
       <c r="H9" t="n">
-        <v>3.4</v>
+        <v>31.37</v>
       </c>
       <c r="I9" t="n">
-        <v>3.69</v>
+        <v>38.14</v>
       </c>
       <c r="J9" t="n">
-        <v>3.93</v>
+        <v>45.26</v>
       </c>
       <c r="K9" t="n">
-        <v>4.12</v>
+        <v>52.6</v>
       </c>
       <c r="L9" t="n">
-        <v>4.22</v>
+        <v>60.06</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7000</v>
+        <v>23359</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6899999999999999</v>
+        <v>3.37</v>
       </c>
       <c r="C10" t="n">
-        <v>1.25</v>
+        <v>6.46</v>
       </c>
       <c r="D10" t="n">
-        <v>1.81</v>
+        <v>10.43</v>
       </c>
       <c r="E10" t="n">
-        <v>2.32</v>
+        <v>15.23</v>
       </c>
       <c r="F10" t="n">
-        <v>2.78</v>
+        <v>20.8</v>
       </c>
       <c r="G10" t="n">
-        <v>3.19</v>
+        <v>27.04</v>
       </c>
       <c r="H10" t="n">
-        <v>3.55</v>
+        <v>33.86</v>
       </c>
       <c r="I10" t="n">
-        <v>3.86</v>
+        <v>41.17</v>
       </c>
       <c r="J10" t="n">
-        <v>4.12</v>
+        <v>48.85</v>
       </c>
       <c r="K10" t="n">
-        <v>4.33</v>
+        <v>56.78</v>
       </c>
       <c r="L10" t="n">
-        <v>4.44</v>
+        <v>64.84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7500</v>
+        <v>26154</v>
       </c>
       <c r="B11" t="n">
-        <v>0.72</v>
+        <v>3.61</v>
       </c>
       <c r="C11" t="n">
-        <v>1.3</v>
+        <v>6.91</v>
       </c>
       <c r="D11" t="n">
-        <v>1.88</v>
+        <v>11.16</v>
       </c>
       <c r="E11" t="n">
-        <v>2.41</v>
+        <v>16.3</v>
       </c>
       <c r="F11" t="n">
-        <v>2.89</v>
+        <v>22.26</v>
       </c>
       <c r="G11" t="n">
-        <v>3.32</v>
+        <v>28.93</v>
       </c>
       <c r="H11" t="n">
-        <v>3.7</v>
+        <v>36.24</v>
       </c>
       <c r="I11" t="n">
-        <v>4.03</v>
+        <v>44.06</v>
       </c>
       <c r="J11" t="n">
-        <v>4.31</v>
+        <v>52.28</v>
       </c>
       <c r="K11" t="n">
-        <v>4.54</v>
+        <v>60.77</v>
       </c>
       <c r="L11" t="n">
-        <v>4.66</v>
+        <v>69.38</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>8000</v>
+        <v>28949</v>
       </c>
       <c r="B12" t="n">
-        <v>0.75</v>
+        <v>3.83</v>
       </c>
       <c r="C12" t="n">
-        <v>1.35</v>
+        <v>7.35</v>
       </c>
       <c r="D12" t="n">
-        <v>1.95</v>
+        <v>11.87</v>
       </c>
       <c r="E12" t="n">
-        <v>2.5</v>
+        <v>17.33</v>
       </c>
       <c r="F12" t="n">
-        <v>3</v>
+        <v>23.65</v>
       </c>
       <c r="G12" t="n">
-        <v>3.45</v>
+        <v>30.75</v>
       </c>
       <c r="H12" t="n">
-        <v>3.85</v>
+        <v>38.52</v>
       </c>
       <c r="I12" t="n">
-        <v>4.2</v>
+        <v>46.83</v>
       </c>
       <c r="J12" t="n">
-        <v>4.5</v>
+        <v>55.57</v>
       </c>
       <c r="K12" t="n">
-        <v>4.75</v>
+        <v>64.58</v>
       </c>
       <c r="L12" t="n">
-        <v>4.88</v>
+        <v>73.73999999999999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>8500</v>
+        <v>31744</v>
       </c>
       <c r="B13" t="n">
-        <v>0.78</v>
+        <v>4.05</v>
       </c>
       <c r="C13" t="n">
-        <v>1.4</v>
+        <v>7.76</v>
       </c>
       <c r="D13" t="n">
-        <v>2.02</v>
+        <v>12.54</v>
       </c>
       <c r="E13" t="n">
-        <v>2.59</v>
+        <v>18.31</v>
       </c>
       <c r="F13" t="n">
-        <v>3.11</v>
+        <v>25</v>
       </c>
       <c r="G13" t="n">
-        <v>3.58</v>
+        <v>32.5</v>
       </c>
       <c r="H13" t="n">
-        <v>4</v>
+        <v>40.71</v>
       </c>
       <c r="I13" t="n">
-        <v>4.37</v>
+        <v>49.49</v>
       </c>
       <c r="J13" t="n">
-        <v>4.69</v>
+        <v>58.73</v>
       </c>
       <c r="K13" t="n">
-        <v>4.96</v>
+        <v>68.26000000000001</v>
       </c>
       <c r="L13" t="n">
-        <v>5.1</v>
+        <v>77.94</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>9000</v>
+        <v>34538</v>
       </c>
       <c r="B14" t="n">
-        <v>0.8100000000000001</v>
+        <v>4.26</v>
       </c>
       <c r="C14" t="n">
-        <v>1.45</v>
+        <v>8.17</v>
       </c>
       <c r="D14" t="n">
-        <v>2.09</v>
+        <v>13.19</v>
       </c>
       <c r="E14" t="n">
-        <v>2.68</v>
+        <v>19.26</v>
       </c>
       <c r="F14" t="n">
-        <v>3.22</v>
+        <v>26.3</v>
       </c>
       <c r="G14" t="n">
-        <v>3.71</v>
+        <v>34.19</v>
       </c>
       <c r="H14" t="n">
-        <v>4.15</v>
+        <v>42.82</v>
       </c>
       <c r="I14" t="n">
-        <v>4.54</v>
+        <v>52.06</v>
       </c>
       <c r="J14" t="n">
-        <v>4.88</v>
+        <v>61.77</v>
       </c>
       <c r="K14" t="n">
-        <v>5.17</v>
+        <v>71.8</v>
       </c>
       <c r="L14" t="n">
-        <v>5.32</v>
+        <v>81.98</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>9500</v>
+        <v>37333</v>
       </c>
       <c r="B15" t="n">
-        <v>0.84</v>
+        <v>4.47</v>
       </c>
       <c r="C15" t="n">
-        <v>1.5</v>
+        <v>8.56</v>
       </c>
       <c r="D15" t="n">
-        <v>2.16</v>
+        <v>13.82</v>
       </c>
       <c r="E15" t="n">
-        <v>2.77</v>
+        <v>20.18</v>
       </c>
       <c r="F15" t="n">
-        <v>3.33</v>
+        <v>27.55</v>
       </c>
       <c r="G15" t="n">
-        <v>3.84</v>
+        <v>35.82</v>
       </c>
       <c r="H15" t="n">
-        <v>4.3</v>
+        <v>44.87</v>
       </c>
       <c r="I15" t="n">
-        <v>4.71</v>
+        <v>54.55</v>
       </c>
       <c r="J15" t="n">
-        <v>5.07</v>
+        <v>64.73</v>
       </c>
       <c r="K15" t="n">
-        <v>5.38</v>
+        <v>75.23</v>
       </c>
       <c r="L15" t="n">
-        <v>5.54</v>
+        <v>85.90000000000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>10000</v>
+        <v>40128</v>
       </c>
       <c r="B16" t="n">
-        <v>0.87</v>
+        <v>4.66</v>
       </c>
       <c r="C16" t="n">
-        <v>1.55</v>
+        <v>8.94</v>
       </c>
       <c r="D16" t="n">
-        <v>2.23</v>
+        <v>14.43</v>
       </c>
       <c r="E16" t="n">
-        <v>2.86</v>
+        <v>21.08</v>
       </c>
       <c r="F16" t="n">
-        <v>3.44</v>
+        <v>28.77</v>
       </c>
       <c r="G16" t="n">
-        <v>3.97</v>
+        <v>37.41</v>
       </c>
       <c r="H16" t="n">
-        <v>4.45</v>
+        <v>46.85</v>
       </c>
       <c r="I16" t="n">
-        <v>4.88</v>
+        <v>56.97</v>
       </c>
       <c r="J16" t="n">
-        <v>5.26</v>
+        <v>67.59</v>
       </c>
       <c r="K16" t="n">
-        <v>5.59</v>
+        <v>78.56</v>
       </c>
       <c r="L16" t="n">
-        <v>5.76</v>
+        <v>89.7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>10500</v>
+        <v>42923</v>
       </c>
       <c r="B17" t="n">
-        <v>0.9</v>
+        <v>4.86</v>
       </c>
       <c r="C17" t="n">
-        <v>1.6</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>2.3</v>
+        <v>15.03</v>
       </c>
       <c r="E17" t="n">
-        <v>2.95</v>
+        <v>21.95</v>
       </c>
       <c r="F17" t="n">
-        <v>3.55</v>
+        <v>29.96</v>
       </c>
       <c r="G17" t="n">
-        <v>4.1</v>
+        <v>38.95</v>
       </c>
       <c r="H17" t="n">
-        <v>4.6</v>
+        <v>48.78</v>
       </c>
       <c r="I17" t="n">
-        <v>5.05</v>
+        <v>59.32</v>
       </c>
       <c r="J17" t="n">
-        <v>5.45</v>
+        <v>70.38</v>
       </c>
       <c r="K17" t="n">
-        <v>5.8</v>
+        <v>81.8</v>
       </c>
       <c r="L17" t="n">
-        <v>5.98</v>
+        <v>93.40000000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>11000</v>
+        <v>45718</v>
       </c>
       <c r="B18" t="n">
-        <v>0.93</v>
+        <v>5.04</v>
       </c>
       <c r="C18" t="n">
-        <v>1.65</v>
+        <v>9.66</v>
       </c>
       <c r="D18" t="n">
-        <v>2.37</v>
+        <v>15.61</v>
       </c>
       <c r="E18" t="n">
-        <v>3.04</v>
+        <v>22.79</v>
       </c>
       <c r="F18" t="n">
-        <v>3.66</v>
+        <v>31.11</v>
       </c>
       <c r="G18" t="n">
-        <v>4.23</v>
+        <v>40.45</v>
       </c>
       <c r="H18" t="n">
-        <v>4.75</v>
+        <v>50.67</v>
       </c>
       <c r="I18" t="n">
-        <v>5.22</v>
+        <v>61.6</v>
       </c>
       <c r="J18" t="n">
-        <v>5.64</v>
+        <v>73.09</v>
       </c>
       <c r="K18" t="n">
-        <v>6.01</v>
+        <v>84.95999999999999</v>
       </c>
       <c r="L18" t="n">
-        <v>6.2</v>
+        <v>97.01000000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>11500</v>
+        <v>48513</v>
       </c>
       <c r="B19" t="n">
-        <v>0.96</v>
+        <v>5.23</v>
       </c>
       <c r="C19" t="n">
-        <v>1.7</v>
+        <v>10.01</v>
       </c>
       <c r="D19" t="n">
-        <v>2.44</v>
+        <v>16.17</v>
       </c>
       <c r="E19" t="n">
-        <v>3.13</v>
+        <v>23.62</v>
       </c>
       <c r="F19" t="n">
-        <v>3.77</v>
+        <v>32.24</v>
       </c>
       <c r="G19" t="n">
-        <v>4.36</v>
+        <v>41.92</v>
       </c>
       <c r="H19" t="n">
-        <v>4.9</v>
+        <v>52.5</v>
       </c>
       <c r="I19" t="n">
-        <v>5.39</v>
+        <v>63.84</v>
       </c>
       <c r="J19" t="n">
-        <v>5.83</v>
+        <v>75.73999999999999</v>
       </c>
       <c r="K19" t="n">
-        <v>6.22</v>
+        <v>88.04000000000001</v>
       </c>
       <c r="L19" t="n">
-        <v>6.42</v>
+        <v>100.52</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>12000</v>
+        <v>51308</v>
       </c>
       <c r="B20" t="n">
-        <v>0.99</v>
+        <v>5.4</v>
       </c>
       <c r="C20" t="n">
-        <v>1.75</v>
+        <v>10.36</v>
       </c>
       <c r="D20" t="n">
-        <v>2.51</v>
+        <v>16.73</v>
       </c>
       <c r="E20" t="n">
-        <v>3.22</v>
+        <v>24.43</v>
       </c>
       <c r="F20" t="n">
-        <v>3.88</v>
+        <v>33.34</v>
       </c>
       <c r="G20" t="n">
-        <v>4.49</v>
+        <v>43.35</v>
       </c>
       <c r="H20" t="n">
-        <v>5.05</v>
+        <v>54.3</v>
       </c>
       <c r="I20" t="n">
-        <v>5.56</v>
+        <v>66.02</v>
       </c>
       <c r="J20" t="n">
-        <v>6.02</v>
+        <v>78.33</v>
       </c>
       <c r="K20" t="n">
-        <v>6.43</v>
+        <v>91.05</v>
       </c>
       <c r="L20" t="n">
-        <v>6.64</v>
+        <v>103.96</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>12500</v>
+        <v>54103</v>
       </c>
       <c r="B21" t="n">
-        <v>1.02</v>
+        <v>5.58</v>
       </c>
       <c r="C21" t="n">
-        <v>1.8</v>
+        <v>10.69</v>
       </c>
       <c r="D21" t="n">
-        <v>2.58</v>
+        <v>17.27</v>
       </c>
       <c r="E21" t="n">
-        <v>3.31</v>
+        <v>25.22</v>
       </c>
       <c r="F21" t="n">
-        <v>3.99</v>
+        <v>34.42</v>
       </c>
       <c r="G21" t="n">
-        <v>4.62</v>
+        <v>44.75</v>
       </c>
       <c r="H21" t="n">
-        <v>5.2</v>
+        <v>56.05</v>
       </c>
       <c r="I21" t="n">
-        <v>5.73</v>
+        <v>68.15000000000001</v>
       </c>
       <c r="J21" t="n">
-        <v>6.21</v>
+        <v>80.87</v>
       </c>
       <c r="K21" t="n">
-        <v>6.64</v>
+        <v>93.98999999999999</v>
       </c>
       <c r="L21" t="n">
-        <v>6.86</v>
+        <v>107.32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>13000</v>
+        <v>56897</v>
       </c>
       <c r="B22" t="n">
-        <v>1.05</v>
+        <v>5.75</v>
       </c>
       <c r="C22" t="n">
-        <v>1.85</v>
+        <v>11.02</v>
       </c>
       <c r="D22" t="n">
-        <v>2.65</v>
+        <v>17.8</v>
       </c>
       <c r="E22" t="n">
-        <v>3.4</v>
+        <v>25.99</v>
       </c>
       <c r="F22" t="n">
-        <v>4.1</v>
+        <v>35.48</v>
       </c>
       <c r="G22" t="n">
-        <v>4.75</v>
+        <v>46.13</v>
       </c>
       <c r="H22" t="n">
-        <v>5.35</v>
+        <v>57.77</v>
       </c>
       <c r="I22" t="n">
-        <v>5.9</v>
+        <v>70.23999999999999</v>
       </c>
       <c r="J22" t="n">
-        <v>6.4</v>
+        <v>83.34999999999999</v>
       </c>
       <c r="K22" t="n">
-        <v>6.85</v>
+        <v>96.87</v>
       </c>
       <c r="L22" t="n">
-        <v>7.08</v>
+        <v>110.61</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>13500</v>
+        <v>59692</v>
       </c>
       <c r="B23" t="n">
-        <v>1.08</v>
+        <v>5.92</v>
       </c>
       <c r="C23" t="n">
-        <v>1.9</v>
+        <v>11.34</v>
       </c>
       <c r="D23" t="n">
-        <v>2.72</v>
+        <v>18.32</v>
       </c>
       <c r="E23" t="n">
-        <v>3.49</v>
+        <v>26.75</v>
       </c>
       <c r="F23" t="n">
-        <v>4.21</v>
+        <v>36.51</v>
       </c>
       <c r="G23" t="n">
-        <v>4.88</v>
+        <v>47.47</v>
       </c>
       <c r="H23" t="n">
-        <v>5.5</v>
+        <v>59.46</v>
       </c>
       <c r="I23" t="n">
-        <v>6.07</v>
+        <v>72.29000000000001</v>
       </c>
       <c r="J23" t="n">
-        <v>6.59</v>
+        <v>85.78</v>
       </c>
       <c r="K23" t="n">
-        <v>7.06</v>
+        <v>99.7</v>
       </c>
       <c r="L23" t="n">
-        <v>7.3</v>
+        <v>113.84</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>14000</v>
+        <v>62487</v>
       </c>
       <c r="B24" t="n">
-        <v>1.11</v>
+        <v>6.08</v>
       </c>
       <c r="C24" t="n">
-        <v>1.95</v>
+        <v>11.66</v>
       </c>
       <c r="D24" t="n">
-        <v>2.79</v>
+        <v>18.83</v>
       </c>
       <c r="E24" t="n">
-        <v>3.58</v>
+        <v>27.49</v>
       </c>
       <c r="F24" t="n">
-        <v>4.32</v>
+        <v>37.53</v>
       </c>
       <c r="G24" t="n">
-        <v>5.01</v>
+        <v>48.79</v>
       </c>
       <c r="H24" t="n">
-        <v>5.65</v>
+        <v>61.11</v>
       </c>
       <c r="I24" t="n">
-        <v>6.24</v>
+        <v>74.31</v>
       </c>
       <c r="J24" t="n">
-        <v>6.78</v>
+        <v>88.17</v>
       </c>
       <c r="K24" t="n">
-        <v>7.27</v>
+        <v>102.48</v>
       </c>
       <c r="L24" t="n">
-        <v>7.52</v>
+        <v>117.01</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>14500</v>
+        <v>65282</v>
       </c>
       <c r="B25" t="n">
-        <v>1.14</v>
+        <v>6.24</v>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>11.97</v>
       </c>
       <c r="D25" t="n">
-        <v>2.86</v>
+        <v>19.33</v>
       </c>
       <c r="E25" t="n">
-        <v>3.67</v>
+        <v>28.22</v>
       </c>
       <c r="F25" t="n">
-        <v>4.43</v>
+        <v>38.53</v>
       </c>
       <c r="G25" t="n">
-        <v>5.14</v>
+        <v>50.09</v>
       </c>
       <c r="H25" t="n">
-        <v>5.8</v>
+        <v>62.74</v>
       </c>
       <c r="I25" t="n">
-        <v>6.41</v>
+        <v>76.28</v>
       </c>
       <c r="J25" t="n">
-        <v>6.97</v>
+        <v>90.51000000000001</v>
       </c>
       <c r="K25" t="n">
-        <v>7.48</v>
+        <v>105.2</v>
       </c>
       <c r="L25" t="n">
-        <v>7.74</v>
+        <v>120.12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>15000</v>
+        <v>68077</v>
       </c>
       <c r="B26" t="n">
-        <v>1.17</v>
+        <v>6.4</v>
       </c>
       <c r="C26" t="n">
-        <v>2.05</v>
+        <v>12.27</v>
       </c>
       <c r="D26" t="n">
-        <v>2.93</v>
+        <v>19.82</v>
       </c>
       <c r="E26" t="n">
-        <v>3.76</v>
+        <v>28.94</v>
       </c>
       <c r="F26" t="n">
-        <v>4.54</v>
+        <v>39.51</v>
       </c>
       <c r="G26" t="n">
-        <v>5.27</v>
+        <v>51.37</v>
       </c>
       <c r="H26" t="n">
-        <v>5.95</v>
+        <v>64.34</v>
       </c>
       <c r="I26" t="n">
-        <v>6.58</v>
+        <v>78.23</v>
       </c>
       <c r="J26" t="n">
-        <v>7.16</v>
+        <v>92.81999999999999</v>
       </c>
       <c r="K26" t="n">
-        <v>7.69</v>
+        <v>107.88</v>
       </c>
       <c r="L26" t="n">
-        <v>7.96</v>
+        <v>123.18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>15500</v>
+        <v>70872</v>
       </c>
       <c r="B27" t="n">
-        <v>1.2</v>
+        <v>6.56</v>
       </c>
       <c r="C27" t="n">
-        <v>2.1</v>
+        <v>12.57</v>
       </c>
       <c r="D27" t="n">
-        <v>3</v>
+        <v>20.3</v>
       </c>
       <c r="E27" t="n">
-        <v>3.85</v>
+        <v>29.65</v>
       </c>
       <c r="F27" t="n">
-        <v>4.65</v>
+        <v>40.48</v>
       </c>
       <c r="G27" t="n">
-        <v>5.4</v>
+        <v>52.62</v>
       </c>
       <c r="H27" t="n">
-        <v>6.1</v>
+        <v>65.91</v>
       </c>
       <c r="I27" t="n">
-        <v>6.75</v>
+        <v>80.14</v>
       </c>
       <c r="J27" t="n">
-        <v>7.35</v>
+        <v>95.09</v>
       </c>
       <c r="K27" t="n">
-        <v>7.9</v>
+        <v>110.52</v>
       </c>
       <c r="L27" t="n">
-        <v>8.18</v>
+        <v>126.19</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>16000</v>
+        <v>73667</v>
       </c>
       <c r="B28" t="n">
-        <v>1.23</v>
+        <v>6.71</v>
       </c>
       <c r="C28" t="n">
-        <v>2.15</v>
+        <v>12.87</v>
       </c>
       <c r="D28" t="n">
-        <v>3.07</v>
+        <v>20.78</v>
       </c>
       <c r="E28" t="n">
-        <v>3.94</v>
+        <v>30.35</v>
       </c>
       <c r="F28" t="n">
-        <v>4.76</v>
+        <v>41.43</v>
       </c>
       <c r="G28" t="n">
-        <v>5.53</v>
+        <v>53.86</v>
       </c>
       <c r="H28" t="n">
-        <v>6.25</v>
+        <v>67.45999999999999</v>
       </c>
       <c r="I28" t="n">
-        <v>6.92</v>
+        <v>82.02</v>
       </c>
       <c r="J28" t="n">
-        <v>7.54</v>
+        <v>97.31999999999999</v>
       </c>
       <c r="K28" t="n">
-        <v>8.109999999999999</v>
+        <v>113.11</v>
       </c>
       <c r="L28" t="n">
-        <v>8.4</v>
+        <v>129.15</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>16500</v>
+        <v>76462</v>
       </c>
       <c r="B29" t="n">
-        <v>1.26</v>
+        <v>6.87</v>
       </c>
       <c r="C29" t="n">
-        <v>2.2</v>
+        <v>13.16</v>
       </c>
       <c r="D29" t="n">
-        <v>3.14</v>
+        <v>21.25</v>
       </c>
       <c r="E29" t="n">
-        <v>4.03</v>
+        <v>31.03</v>
       </c>
       <c r="F29" t="n">
-        <v>4.87</v>
+        <v>42.36</v>
       </c>
       <c r="G29" t="n">
-        <v>5.66</v>
+        <v>55.08</v>
       </c>
       <c r="H29" t="n">
-        <v>6.4</v>
+        <v>68.98</v>
       </c>
       <c r="I29" t="n">
-        <v>7.09</v>
+        <v>83.87</v>
       </c>
       <c r="J29" t="n">
-        <v>7.73</v>
+        <v>99.52</v>
       </c>
       <c r="K29" t="n">
-        <v>8.32</v>
+        <v>115.67</v>
       </c>
       <c r="L29" t="n">
-        <v>8.619999999999999</v>
+        <v>132.07</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>17000</v>
+        <v>79256</v>
       </c>
       <c r="B30" t="n">
-        <v>1.29</v>
+        <v>7.02</v>
       </c>
       <c r="C30" t="n">
-        <v>2.25</v>
+        <v>13.44</v>
       </c>
       <c r="D30" t="n">
-        <v>3.21</v>
+        <v>21.71</v>
       </c>
       <c r="E30" t="n">
-        <v>4.12</v>
+        <v>31.71</v>
       </c>
       <c r="F30" t="n">
-        <v>4.98</v>
+        <v>43.28</v>
       </c>
       <c r="G30" t="n">
-        <v>5.79</v>
+        <v>56.27</v>
       </c>
       <c r="H30" t="n">
-        <v>6.55</v>
+        <v>70.48</v>
       </c>
       <c r="I30" t="n">
-        <v>7.26</v>
+        <v>85.7</v>
       </c>
       <c r="J30" t="n">
-        <v>7.92</v>
+        <v>101.68</v>
       </c>
       <c r="K30" t="n">
-        <v>8.529999999999999</v>
+        <v>118.19</v>
       </c>
       <c r="L30" t="n">
-        <v>8.84</v>
+        <v>134.95</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>17500</v>
+        <v>82051</v>
       </c>
       <c r="B31" t="n">
-        <v>1.32</v>
+        <v>7.16</v>
       </c>
       <c r="C31" t="n">
-        <v>2.3</v>
+        <v>13.73</v>
       </c>
       <c r="D31" t="n">
-        <v>3.28</v>
+        <v>22.17</v>
       </c>
       <c r="E31" t="n">
-        <v>4.21</v>
+        <v>32.37</v>
       </c>
       <c r="F31" t="n">
-        <v>5.09</v>
+        <v>44.19</v>
       </c>
       <c r="G31" t="n">
-        <v>5.92</v>
+        <v>57.46</v>
       </c>
       <c r="H31" t="n">
-        <v>6.7</v>
+        <v>71.95999999999999</v>
       </c>
       <c r="I31" t="n">
-        <v>7.43</v>
+        <v>87.5</v>
       </c>
       <c r="J31" t="n">
-        <v>8.109999999999999</v>
+        <v>103.82</v>
       </c>
       <c r="K31" t="n">
-        <v>8.74</v>
+        <v>120.67</v>
       </c>
       <c r="L31" t="n">
-        <v>9.06</v>
+        <v>137.78</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>18000</v>
+        <v>84846</v>
       </c>
       <c r="B32" t="n">
-        <v>1.35</v>
+        <v>7.31</v>
       </c>
       <c r="C32" t="n">
-        <v>2.35</v>
+        <v>14</v>
       </c>
       <c r="D32" t="n">
-        <v>3.35</v>
+        <v>22.62</v>
       </c>
       <c r="E32" t="n">
-        <v>4.3</v>
+        <v>33.03</v>
       </c>
       <c r="F32" t="n">
-        <v>5.2</v>
+        <v>45.09</v>
       </c>
       <c r="G32" t="n">
-        <v>6.05</v>
+        <v>58.62</v>
       </c>
       <c r="H32" t="n">
-        <v>6.85</v>
+        <v>73.43000000000001</v>
       </c>
       <c r="I32" t="n">
-        <v>7.6</v>
+        <v>89.28</v>
       </c>
       <c r="J32" t="n">
-        <v>8.300000000000001</v>
+        <v>105.93</v>
       </c>
       <c r="K32" t="n">
-        <v>8.949999999999999</v>
+        <v>123.12</v>
       </c>
       <c r="L32" t="n">
-        <v>9.279999999999999</v>
+        <v>140.58</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>18500</v>
+        <v>87641</v>
       </c>
       <c r="B33" t="n">
-        <v>1.38</v>
+        <v>7.45</v>
       </c>
       <c r="C33" t="n">
-        <v>2.4</v>
+        <v>14.28</v>
       </c>
       <c r="D33" t="n">
-        <v>3.42</v>
+        <v>23.06</v>
       </c>
       <c r="E33" t="n">
-        <v>4.39</v>
+        <v>33.68</v>
       </c>
       <c r="F33" t="n">
-        <v>5.31</v>
+        <v>45.98</v>
       </c>
       <c r="G33" t="n">
-        <v>6.18</v>
+        <v>59.77</v>
       </c>
       <c r="H33" t="n">
-        <v>7</v>
+        <v>74.87</v>
       </c>
       <c r="I33" t="n">
-        <v>7.77</v>
+        <v>91.03</v>
       </c>
       <c r="J33" t="n">
-        <v>8.49</v>
+        <v>108.01</v>
       </c>
       <c r="K33" t="n">
-        <v>9.16</v>
+        <v>125.54</v>
       </c>
       <c r="L33" t="n">
-        <v>9.5</v>
+        <v>143.34</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>90436</v>
+      </c>
+      <c r="B34" t="n">
+        <v>7.59</v>
+      </c>
+      <c r="C34" t="n">
+        <v>14.55</v>
+      </c>
+      <c r="D34" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E34" t="n">
+        <v>34.32</v>
+      </c>
+      <c r="F34" t="n">
+        <v>46.85</v>
+      </c>
+      <c r="G34" t="n">
+        <v>60.91</v>
+      </c>
+      <c r="H34" t="n">
+        <v>76.29000000000001</v>
+      </c>
+      <c r="I34" t="n">
+        <v>92.76000000000001</v>
+      </c>
+      <c r="J34" t="n">
+        <v>110.06</v>
+      </c>
+      <c r="K34" t="n">
+        <v>127.93</v>
+      </c>
+      <c r="L34" t="n">
+        <v>146.07</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>93231</v>
+      </c>
+      <c r="B35" t="n">
+        <v>7.73</v>
+      </c>
+      <c r="C35" t="n">
+        <v>14.82</v>
+      </c>
+      <c r="D35" t="n">
+        <v>23.93</v>
+      </c>
+      <c r="E35" t="n">
+        <v>34.95</v>
+      </c>
+      <c r="F35" t="n">
+        <v>47.71</v>
+      </c>
+      <c r="G35" t="n">
+        <v>62.03</v>
+      </c>
+      <c r="H35" t="n">
+        <v>77.7</v>
+      </c>
+      <c r="I35" t="n">
+        <v>94.47</v>
+      </c>
+      <c r="J35" t="n">
+        <v>112.09</v>
+      </c>
+      <c r="K35" t="n">
+        <v>130.28</v>
+      </c>
+      <c r="L35" t="n">
+        <v>148.76</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>96026</v>
+      </c>
+      <c r="B36" t="n">
+        <v>7.87</v>
+      </c>
+      <c r="C36" t="n">
+        <v>15.08</v>
+      </c>
+      <c r="D36" t="n">
+        <v>24.36</v>
+      </c>
+      <c r="E36" t="n">
+        <v>35.58</v>
+      </c>
+      <c r="F36" t="n">
+        <v>48.57</v>
+      </c>
+      <c r="G36" t="n">
+        <v>63.14</v>
+      </c>
+      <c r="H36" t="n">
+        <v>79.09</v>
+      </c>
+      <c r="I36" t="n">
+        <v>96.16</v>
+      </c>
+      <c r="J36" t="n">
+        <v>114.09</v>
+      </c>
+      <c r="K36" t="n">
+        <v>132.61</v>
+      </c>
+      <c r="L36" t="n">
+        <v>151.42</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>98821</v>
+      </c>
+      <c r="B37" t="n">
+        <v>8.01</v>
+      </c>
+      <c r="C37" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="D37" t="n">
+        <v>24.79</v>
+      </c>
+      <c r="E37" t="n">
+        <v>36.2</v>
+      </c>
+      <c r="F37" t="n">
+        <v>49.41</v>
+      </c>
+      <c r="G37" t="n">
+        <v>64.23999999999999</v>
+      </c>
+      <c r="H37" t="n">
+        <v>80.45999999999999</v>
+      </c>
+      <c r="I37" t="n">
+        <v>97.83</v>
+      </c>
+      <c r="J37" t="n">
+        <v>116.08</v>
+      </c>
+      <c r="K37" t="n">
+        <v>134.92</v>
+      </c>
+      <c r="L37" t="n">
+        <v>154.05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>101615</v>
+      </c>
+      <c r="B38" t="n">
+        <v>8.140000000000001</v>
+      </c>
+      <c r="C38" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="D38" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="E38" t="n">
+        <v>36.81</v>
+      </c>
+      <c r="F38" t="n">
+        <v>50.24</v>
+      </c>
+      <c r="G38" t="n">
+        <v>65.31999999999999</v>
+      </c>
+      <c r="H38" t="n">
+        <v>81.81999999999999</v>
+      </c>
+      <c r="I38" t="n">
+        <v>99.48</v>
+      </c>
+      <c r="J38" t="n">
+        <v>118.03</v>
+      </c>
+      <c r="K38" t="n">
+        <v>137.19</v>
+      </c>
+      <c r="L38" t="n">
+        <v>156.65</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>104410</v>
+      </c>
+      <c r="B39" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="C39" t="n">
+        <v>15.86</v>
+      </c>
+      <c r="D39" t="n">
+        <v>25.62</v>
+      </c>
+      <c r="E39" t="n">
+        <v>37.41</v>
+      </c>
+      <c r="F39" t="n">
+        <v>51.07</v>
+      </c>
+      <c r="G39" t="n">
+        <v>66.39</v>
+      </c>
+      <c r="H39" t="n">
+        <v>83.16</v>
+      </c>
+      <c r="I39" t="n">
+        <v>101.11</v>
+      </c>
+      <c r="J39" t="n">
+        <v>119.97</v>
+      </c>
+      <c r="K39" t="n">
+        <v>139.44</v>
+      </c>
+      <c r="L39" t="n">
+        <v>159.22</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>107205</v>
+      </c>
+      <c r="B40" t="n">
+        <v>8.41</v>
+      </c>
+      <c r="C40" t="n">
+        <v>16.11</v>
+      </c>
+      <c r="D40" t="n">
+        <v>26.03</v>
+      </c>
+      <c r="E40" t="n">
+        <v>38.01</v>
+      </c>
+      <c r="F40" t="n">
+        <v>51.88</v>
+      </c>
+      <c r="G40" t="n">
+        <v>67.45999999999999</v>
+      </c>
+      <c r="H40" t="n">
+        <v>84.48999999999999</v>
+      </c>
+      <c r="I40" t="n">
+        <v>102.73</v>
+      </c>
+      <c r="J40" t="n">
+        <v>121.89</v>
+      </c>
+      <c r="K40" t="n">
+        <v>141.67</v>
+      </c>
+      <c r="L40" t="n">
+        <v>161.76</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>110000</v>
+      </c>
+      <c r="B41" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="C41" t="n">
+        <v>16.37</v>
+      </c>
+      <c r="D41" t="n">
+        <v>26.43</v>
+      </c>
+      <c r="E41" t="n">
+        <v>38.6</v>
+      </c>
+      <c r="F41" t="n">
+        <v>52.69</v>
+      </c>
+      <c r="G41" t="n">
+        <v>68.51000000000001</v>
+      </c>
+      <c r="H41" t="n">
+        <v>85.8</v>
+      </c>
+      <c r="I41" t="n">
+        <v>104.33</v>
+      </c>
+      <c r="J41" t="n">
+        <v>123.78</v>
+      </c>
+      <c r="K41" t="n">
+        <v>143.88</v>
+      </c>
+      <c r="L41" t="n">
+        <v>164.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrate actual MV Del Monte KN curves from extracted data
Co-authored-by: tanmegan05-droid <253447754+tanmegan05-droid@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/MV_Del_Monte_Ship_Data.xlsx
+++ b/data/MV_Del_Monte_Ship_Data.xlsx
@@ -10246,7 +10246,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10257,1963 +10257,557 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Displacement (tonnes)</t>
+          <t>Displacement</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>KN at 10°</t>
+          <t>5°</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>KN at 15°</t>
+          <t>10°</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>KN at 20°</t>
+          <t>12°</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>KN at 25°</t>
+          <t>15°</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>KN at 30°</t>
+          <t>20°</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>KN at 35°</t>
+          <t>25°</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>KN at 40°</t>
+          <t>30°</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>KN at 45°</t>
+          <t>35°</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>KN at 50°</t>
+          <t>40°</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>KN at 55°</t>
+          <t>50°</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>KN at 60°</t>
+          <t>60°</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>75°</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>90°</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2206</v>
+        <v>10000</v>
       </c>
       <c r="B2" t="n">
-        <v>0.05665049282421264</v>
+        <v>3.5</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08443639693975437</v>
+        <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1115796890904941</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1378737924335969</v>
+        <v>9.9</v>
       </c>
       <c r="F2" t="n">
-        <v>0.163118592965808</v>
+        <v>11.45</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1871219625118499</v>
+        <v>11.85</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2097012209358465</v>
+        <v>11.4</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2306845264474622</v>
+        <v>11</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2499121834216873</v>
+        <v>10.4</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2672378577789711</v>
+        <v>9.4</v>
       </c>
       <c r="L2" t="n">
-        <v>0.2825296906759267</v>
+        <v>8.699999999999999</v>
+      </c>
+      <c r="M2" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>8.6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3864.387755102041</v>
+        <v>20000</v>
       </c>
       <c r="B3" t="n">
-        <v>0.07089143507618116</v>
+        <v>2.15</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1056622291053203</v>
+        <v>4.2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1396288697703696</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1725328504262497</v>
+        <v>6.2</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2041237519122026</v>
+        <v>8</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2341611483928125</v>
+        <v>9.6</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2624164371437858</v>
+        <v>10.75</v>
       </c>
       <c r="I3" t="n">
-        <v>0.288674578356718</v>
+        <v>11.45</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3127357317218794</v>
+        <v>11.85</v>
       </c>
       <c r="K3" t="n">
-        <v>0.3344167773336396</v>
+        <v>11.9</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3535527093435198</v>
+        <v>11.45</v>
+      </c>
+      <c r="M3" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="N3" t="n">
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5522.775510204081</v>
+        <v>30000</v>
       </c>
       <c r="B4" t="n">
-        <v>0.08177573292256292</v>
+        <v>1.6</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1218850516713899</v>
+        <v>3.15</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1610667515807913</v>
+        <v>3.8</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1990226362558992</v>
+        <v>4.7</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2354638384959462</v>
+        <v>6.2</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2701130187480861</v>
+        <v>7.55</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3027064758288532</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3329961538493952</v>
+        <v>9.9</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3607515300705682</v>
+        <v>10.85</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3857613693201747</v>
+        <v>11.75</v>
       </c>
       <c r="L4" t="n">
-        <v>0.4078353316201713</v>
+        <v>11.9</v>
+      </c>
+      <c r="M4" t="n">
+        <v>11.45</v>
+      </c>
+      <c r="N4" t="n">
+        <v>10.8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7181.163265306122</v>
+        <v>40000</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0908321113576769</v>
+        <v>1.4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1353833978686023</v>
+        <v>2.75</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1789043349750169</v>
+        <v>3.3</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2210637020668807</v>
+        <v>4.05</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2615406409041026</v>
+        <v>5.35</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3000270975414877</v>
+        <v>6.55</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3362301668052673</v>
+        <v>7.65</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3698743214783334</v>
+        <v>8.6</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4007035092287279</v>
+        <v>9.550000000000001</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4284831013224976</v>
+        <v>10.9</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4530016782900327</v>
+        <v>11.55</v>
+      </c>
+      <c r="M5" t="n">
+        <v>11.85</v>
+      </c>
+      <c r="N5" t="n">
+        <v>11.45</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>8839.551020408162</v>
+        <v>50000</v>
       </c>
       <c r="B6" t="n">
-        <v>0.09870373156675853</v>
+        <v>1.3</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1471158862442186</v>
+        <v>2.55</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1944084001963592</v>
+        <v>3.05</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2402213488360042</v>
+        <v>3.75</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2842060679613908</v>
+        <v>4.95</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3260278073012755</v>
+        <v>5.95</v>
       </c>
       <c r="H6" t="n">
-        <v>0.365368278166625</v>
+        <v>6.95</v>
       </c>
       <c r="I6" t="n">
-        <v>0.4019280758197284</v>
+        <v>7.85</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4354289581250361</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="K6" t="n">
-        <v>0.4656159631398188</v>
+        <v>10.05</v>
       </c>
       <c r="L6" t="n">
-        <v>0.4922593495285021</v>
+        <v>10.95</v>
+      </c>
+      <c r="M6" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="N6" t="n">
+        <v>11.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>10497.9387755102</v>
+        <v>60000</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1057311858886179</v>
+        <v>1.25</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1575901626893988</v>
+        <v>2.5</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2082497831965717</v>
+        <v>2.95</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2573244971089615</v>
+        <v>3.6</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3044408162215725</v>
+        <v>4.7</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3492401568963467</v>
+        <v>5.6</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3913815691001672</v>
+        <v>6.5</v>
       </c>
       <c r="I7" t="n">
-        <v>0.4305443312404829</v>
+        <v>7.35</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4664303910502834</v>
+        <v>8.15</v>
       </c>
       <c r="K7" t="n">
-        <v>0.4987666339458209</v>
+        <v>9.449999999999999</v>
       </c>
       <c r="L7" t="n">
-        <v>0.527306961593503</v>
+        <v>10.4</v>
+      </c>
+      <c r="M7" t="n">
+        <v>11.15</v>
+      </c>
+      <c r="N7" t="n">
+        <v>11.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>12156.32653061224</v>
+        <v>70000</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1121198303417254</v>
+        <v>1.2</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1671123061352365</v>
+        <v>2.45</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2208329563738891</v>
+        <v>2.9</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2728729344719517</v>
+        <v>3.45</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3228361847735</v>
+        <v>4.5</v>
       </c>
       <c r="G8" t="n">
-        <v>0.370342456775104</v>
+        <v>5.35</v>
       </c>
       <c r="H8" t="n">
-        <v>0.41503019906176</v>
+        <v>6.15</v>
       </c>
       <c r="I8" t="n">
-        <v>0.4565593109314702</v>
+        <v>6.95</v>
       </c>
       <c r="J8" t="n">
-        <v>0.4946137307669427</v>
+        <v>7.7</v>
       </c>
       <c r="K8" t="n">
-        <v>0.5289038414553425</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>0.559168674549396</v>
+        <v>9.85</v>
+      </c>
+      <c r="M8" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="N8" t="n">
+        <v>11.1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>13814.71428571428</v>
+        <v>80000</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1180044138463015</v>
+        <v>1.2</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1758831570819233</v>
+        <v>2.4</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2324233232909977</v>
+        <v>2.85</v>
       </c>
       <c r="E9" t="n">
-        <v>0.287194607668788</v>
+        <v>3.4</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3397801676693734</v>
+        <v>4.35</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3897797954291203</v>
+        <v>5.1</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4368129635901762</v>
+        <v>5.9</v>
       </c>
       <c r="I9" t="n">
-        <v>0.4805217213434321</v>
+        <v>6.65</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5205734186503164</v>
+        <v>7.35</v>
       </c>
       <c r="K9" t="n">
-        <v>0.5566632379104474</v>
+        <v>8.5</v>
       </c>
       <c r="L9" t="n">
-        <v>0.5885165138076268</v>
+        <v>9.4</v>
+      </c>
+      <c r="M9" t="n">
+        <v>10.25</v>
+      </c>
+      <c r="N9" t="n">
+        <v>10.7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>15473.10204081633</v>
+        <v>90000</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1234788126994494</v>
+        <v>1.2</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1840426362237071</v>
+        <v>2.4</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2432057841583202</v>
+        <v>2.85</v>
       </c>
       <c r="E10" t="n">
-        <v>0.300517989223821</v>
+        <v>3.4</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3555430709336053</v>
+        <v>4.25</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4078622551908091</v>
+        <v>5</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4570773614120477</v>
+        <v>5.7</v>
       </c>
       <c r="I10" t="n">
-        <v>0.502813832922084</v>
+        <v>6.4</v>
       </c>
       <c r="J10" t="n">
-        <v>0.54472358755629</v>
+        <v>7.05</v>
       </c>
       <c r="K10" t="n">
-        <v>0.5824876667760978</v>
+        <v>8.15</v>
       </c>
       <c r="L10" t="n">
-        <v>0.6158186631360698</v>
+        <v>9</v>
+      </c>
+      <c r="M10" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="N10" t="n">
+        <v>10.25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>17131.48979591837</v>
+        <v>100000</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1286114225244543</v>
+        <v>1.2</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1916926858334392</v>
+        <v>2.35</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2533150520560232</v>
+        <v>2.8</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3130095377766505</v>
+        <v>3.35</v>
       </c>
       <c r="F11" t="n">
-        <v>0.370321831914471</v>
+        <v>4.15</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4248157533049868</v>
+        <v>4.9</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4760765703020864</v>
+        <v>5.55</v>
       </c>
       <c r="I11" t="n">
-        <v>0.5237141571362945</v>
+        <v>6.2</v>
       </c>
       <c r="J11" t="n">
-        <v>0.5673659630074415</v>
+        <v>6.85</v>
       </c>
       <c r="K11" t="n">
-        <v>0.6066997713151667</v>
+        <v>7.85</v>
       </c>
       <c r="L11" t="n">
-        <v>0.6414162280278456</v>
+        <v>8.65</v>
+      </c>
+      <c r="M11" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="N11" t="n">
+        <v>9.949999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>18789.87755102041</v>
+        <v>110000</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1334538382623365</v>
+        <v>1.2</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1989102071118485</v>
+        <v>2.3</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2628527491799725</v>
+        <v>2.75</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3247948231120076</v>
+        <v>3.25</v>
       </c>
       <c r="F12" t="n">
-        <v>0.384265012323684</v>
+        <v>4.1</v>
       </c>
       <c r="G12" t="n">
-        <v>0.440810712766019</v>
+        <v>4.8</v>
       </c>
       <c r="H12" t="n">
-        <v>0.4940015775154188</v>
+        <v>5.4</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5434327919736184</v>
+        <v>6</v>
       </c>
       <c r="J12" t="n">
-        <v>0.5887281547512075</v>
+        <v>6.65</v>
       </c>
       <c r="K12" t="n">
-        <v>0.6295429407873608</v>
+        <v>7.6</v>
       </c>
       <c r="L12" t="n">
-        <v>0.6655665249157015</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>20448.26530612245</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0.1380460796148254</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.2057548486030552</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.2718976989552412</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.3359712436420586</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.3974878442997763</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.4559793224526504</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.5110005226338171</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.5621327002871889</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.6089867086663705</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.6512059604763726</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.6884691417182398</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>22106.65306122449</v>
-      </c>
-      <c r="B14" t="n">
-        <v>0.1424199035377728</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.212273943398021</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.2805124503744988</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.3466160882255783</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.4100817683527447</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.470426478608605</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.5271909593109798</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.5799431984863934</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.6282817197420482</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.6718386377435913</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.7102824580446447</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>23765.04081632653</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0.1466009939707804</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.2185057728816218</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.2887475909234411</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.3567918654477707</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.4221207384392241</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.4842370177276844</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.5426679609209315</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.5969688732596966</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.6467264920132945</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.6915621316585385</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.731134565905229</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>25423.42857142857</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0.150610460531872</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.2244818005062978</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.2966446984330535</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.3665499510857675</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.4336655372818069</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.4974806668847211</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.5575096682256029</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0.6132956843577464</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.6644141500138684</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.7104760228041523</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.7511307440637448</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>27081.81632653061</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0.1544658947362052</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.230228246064368</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.3042384214243651</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.3759331586931413</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.4447668176296151</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.5102155325263805</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.5717811991440586</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.6289952655853227</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.6814222982577572</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.728663295786417</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.7703587256552145</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>28740.20408163265</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0.1581821332462787</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.2357672232967999</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.3115579824178908</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.3849775971689283</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.4554672999496814</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.5224906215591425</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.5855374740500755</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.6441280328062939</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.6978163882977165</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.7461939397211379</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.7888925046990618</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>30398.59183673469</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0.1617718214903532</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.2411175799548995</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.3186282880452136</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.3937140424704832</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.4658033953015136</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.5343477030345196</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.5988253020994683</v>
-      </c>
-      <c r="I19" t="n">
-        <v>0.6587454790348366</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.7136522051133544</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0.7631276069959766</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0.8067951470003116</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>32056.97959183673</v>
-      </c>
-      <c r="B20" t="n">
-        <v>0.1652458378150658</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.2462955299910772</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.3254707644665494</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.4021689698998104</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.4758064266358704</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.5458227091654561</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.6116849513015298</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0.6728919016127271</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0.7289777382494125</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0.779515614129227</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0.8241209055011212</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>33715.36734693877</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0.16861361805236</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.2513151373191974</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.3321039966428067</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.4103653440220885</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.4855035633479927</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.5569468074017521</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.6241513499575071</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.6866057238671964</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0.7438346136343852</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0.7954024728521967</v>
-      </c>
-      <c r="L21" t="n">
-        <v>0.8409168389744585</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>35373.75510204081</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0.1718834075902471</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.2561886915208739</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.3385442248180656</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.4183232321457998</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.4949185470864307</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.5677472330437447</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.6362550197424436</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0.6999205215596176</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0.7582592055841572</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0.8108270792047748</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0.8572240691618678</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>37032.14285714286</v>
-      </c>
-      <c r="B23" t="n">
-        <v>0.1750624597523426</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.260927003526099</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.3448057352509893</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.4260602871312244</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.5040722629641555</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.5782479445087755</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.6480228100400285</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0.712865830700006</v>
-      </c>
-      <c r="J23" t="n">
-        <v>0.7722835119481993</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0.8258236493529327</v>
-      </c>
-      <c r="L23" t="n">
-        <v>0.8730787701401372</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>38690.5306122449</v>
-      </c>
-      <c r="B24" t="n">
-        <v>0.1781571937954755</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.2655396411054361</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.3509011714093654</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.4335921319189491</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.512983194494542</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.58847014521231</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.6594784827970236</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0.7254677909236567</v>
-      </c>
-      <c r="J24" t="n">
-        <v>0.7859358511119318</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0.8404224649122033</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0.888512956293534</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>40348.91836734694</v>
-      </c>
-      <c r="B25" t="n">
-        <v>0.1811733221103832</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.2700351184600469</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.356841784506567</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.4409326691060317</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0.5216677898511743</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0.5984327037239261</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.6706431833777926</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0.7377496634607285</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0.799241423139302</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0.8546504729926194</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0.903555116694398</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>42007.30612244898</v>
-      </c>
-      <c r="B26" t="n">
-        <v>0.1841159536376892</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.2744210503610813</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0.3626376371912651</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.4480943326358312</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.5301407596422829</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.6081524953601143</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.6815358233757385</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0.7497322522528918</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0.8122227659896893</v>
-      </c>
-      <c r="K26" t="n">
-        <v>0.8685317740437903</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0.9182307308635943</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>43665.69387755102</v>
-      </c>
-      <c r="B27" t="n">
-        <v>0.1869896787028271</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.2787042785943935</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0.3682977706396119</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.4550882942659888</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0.5384153211831763</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.6176446824021004</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0.6921733946438885</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0.7614342494067139</v>
-      </c>
-      <c r="J27" t="n">
-        <v>0.8249001297649841</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0.8820880220474261</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0.932562691862777</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>45324.08163265306</v>
-      </c>
-      <c r="B28" t="n">
-        <v>0.1897986391820535</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0.2828909765415412</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.3738303427553059</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.4619246343357702</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0.5465034005312192</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0.6269229458608502</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0.7025712290260556</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0.7728725209142659</v>
-      </c>
-      <c r="J28" t="n">
-        <v>0.8372917862451313</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0.8953387555120679</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0.9465716562292359</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>46982.4693877551</v>
-      </c>
-      <c r="B29" t="n">
-        <v>0.1925465869759515</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.2869867363333452</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0.3792427433399129</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.4686124840766346</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0.5544158008535788</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0.635999678620614</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0.7127432148062407</v>
-      </c>
-      <c r="I29" t="n">
-        <v>0.7840623447610722</v>
-      </c>
-      <c r="J29" t="n">
-        <v>0.8494142868424841</v>
-      </c>
-      <c r="K29" t="n">
-        <v>0.9083016733106554</v>
-      </c>
-      <c r="L29" t="n">
-        <v>0.9602763355973871</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>48640.85714285714</v>
-      </c>
-      <c r="B30" t="n">
-        <v>0.1952369330798508</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0.290996641988342</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0.3845416907427254</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.4751601450379355</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0.5621623437198667</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0.6448861475231862</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0.7227019783509517</v>
-      </c>
-      <c r="I30" t="n">
-        <v>0.7950176107440812</v>
-      </c>
-      <c r="J30" t="n">
-        <v>0.8612826790746898</v>
-      </c>
-      <c r="K30" t="n">
-        <v>0.9209928661608396</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0.9736937414248081</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>50299.24489795918</v>
-      </c>
-      <c r="B31" t="n">
-        <v>0.1978727890300415</v>
-      </c>
-      <c r="C31" t="n">
-        <v>0.2949253311875151</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0.3897333134938678</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0.4815751899571235</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0.5697519884417552</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0.6535926302686889</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0.7324590375292573</v>
-      </c>
-      <c r="I31" t="n">
-        <v>0.8057509892433692</v>
-      </c>
-      <c r="J31" t="n">
-        <v>0.8729106894035897</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0.9334270121395638</v>
-      </c>
-      <c r="L31" t="n">
-        <v>0.986839391694516</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>51957.63265306122</v>
-      </c>
-      <c r="B32" t="n">
-        <v>0.200457002120952</v>
-      </c>
-      <c r="C32" t="n">
-        <v>0.2987770477647762</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0.3948232196685965</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.4878645484699606</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0.5771929334767997</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0.6621285317412584</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.7420249320750276</v>
-      </c>
-      <c r="I32" t="n">
-        <v>0.8162740746288019</v>
-      </c>
-      <c r="J32" t="n">
-        <v>0.8843108785948889</v>
-      </c>
-      <c r="K32" t="n">
-        <v>0.9456175428133612</v>
-      </c>
-      <c r="L32" t="n">
-        <v>0.9997274865515403</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>53616.02040816326</v>
-      </c>
-      <c r="B33" t="n">
-        <v>0.2029921854970512</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0.3025556865583275</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.3998165561567766</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.4940345803470355</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0.5844927030746176</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0.6705024834054587</v>
-      </c>
-      <c r="H33" t="n">
-        <v>0.7514093349771154</v>
-      </c>
-      <c r="I33" t="n">
-        <v>0.8265975077962348</v>
-      </c>
-      <c r="J33" t="n">
-        <v>0.8954947744678035</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0.9575767851911436</v>
-      </c>
-      <c r="L33" t="n">
-        <v>1.012371058378508</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>55274.4081632653</v>
-      </c>
-      <c r="B34" t="n">
-        <v>0.2054807439997753</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.3062648319349765</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.404718059571391</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.5000911383990213</v>
-      </c>
-      <c r="F34" t="n">
-        <v>0.5916582217001496</v>
-      </c>
-      <c r="G34" t="n">
-        <v>0.678722428681138</v>
-      </c>
-      <c r="H34" t="n">
-        <v>0.7606211481560554</v>
-      </c>
-      <c r="I34" t="n">
-        <v>0.8367310814178991</v>
-      </c>
-      <c r="J34" t="n">
-        <v>0.906472985918112</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0.9693160836521343</v>
-      </c>
-      <c r="L34" t="n">
-        <v>1.02478210070051</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>56932.79591836734</v>
-      </c>
-      <c r="B35" t="n">
-        <v>0.2079248964768675</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0.3099077910417476</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.4095321001893596</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.5060396227722876</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0.5986958782708399</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0.6867956966332962</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0.7696685850457931</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0.8466838307874934</v>
-      </c>
-      <c r="J35" t="n">
-        <v>0.9172553013352261</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0.980845905185904</v>
-      </c>
-      <c r="L35" t="n">
-        <v>1.036971679447167</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>58591.18367346939</v>
-      </c>
-      <c r="B36" t="n">
-        <v>0.2103266951265872</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0.3134876226380303</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0.4142627200521962</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.5118850280280954</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0.6056115818560701</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0.6947290658678491</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0.7785592421994946</v>
-      </c>
-      <c r="I36" t="n">
-        <v>0.8564641125910782</v>
-      </c>
-      <c r="J36" t="n">
-        <v>0.9278507739386733</v>
-      </c>
-      <c r="K36" t="n">
-        <v>0.99217593064498</v>
-      </c>
-      <c r="L36" t="n">
-        <v>1.048950029426872</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>60249.57142857143</v>
-      </c>
-      <c r="B37" t="n">
-        <v>0.2126880423431297</v>
-      </c>
-      <c r="C37" t="n">
-        <v>0.3170071622033305</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0.4189136661450059</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0.5176319841403305</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0.6124108101816094</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0.7025288201736489</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0.7873001616456673</v>
-      </c>
-      <c r="I37" t="n">
-        <v>0.8660796735027272</v>
-      </c>
-      <c r="J37" t="n">
-        <v>0.9382677960912263</v>
-      </c>
-      <c r="K37" t="n">
-        <v>1.003315134209886</v>
-      </c>
-      <c r="L37" t="n">
-        <v>1.060726638338967</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>61907.95918367347</v>
-      </c>
-      <c r="B38" t="n">
-        <v>0.2150107054455049</v>
-      </c>
-      <c r="C38" t="n">
-        <v>0.3204690438903623</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0.4234884194067148</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0.5232847923420832</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0.6190986520397318</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0.7102007971733714</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0.7958978854095555</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0.8755377101614904</v>
-      </c>
-      <c r="J38" t="n">
-        <v>0.9485141642749727</v>
-      </c>
-      <c r="K38" t="n">
-        <v>1.014271852869811</v>
-      </c>
-      <c r="L38" t="n">
-        <v>1.072310320230221</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>63566.34693877551</v>
-      </c>
-      <c r="B39" t="n">
-        <v>0.2172963296050382</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0.3238757197932234</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0.4279902201922757</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0.5288474565881042</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0.625679844512472</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0.7177504310242807</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0.804358503366435</v>
-      </c>
-      <c r="I39" t="n">
-        <v>0.8848449218130274</v>
-      </c>
-      <c r="J39" t="n">
-        <v>0.958597136120651</v>
-      </c>
-      <c r="K39" t="n">
-        <v>1.02505384740562</v>
-      </c>
-      <c r="L39" t="n">
-        <v>1.083709279967397</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>65224.73469387754</v>
-      </c>
-      <c r="B40" t="n">
-        <v>0.2195464492327759</v>
-      </c>
-      <c r="C40" t="n">
-        <v>0.327229476920088</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0.4324220907014778</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0.5343237112690322</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0.6321588057603511</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0.7251827900319108</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0.8126876953939869</v>
-      </c>
-      <c r="I40" t="n">
-        <v>0.8940075566798676</v>
-      </c>
-      <c r="J40" t="n">
-        <v>0.9685234806428928</v>
-      </c>
-      <c r="K40" t="n">
-        <v>1.035668356107759</v>
-      </c>
-      <c r="L40" t="n">
-        <v>1.094931170028993</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>66883.12244897959</v>
-      </c>
-      <c r="B41" t="n">
-        <v>0.221762498044533</v>
-      </c>
-      <c r="C41" t="n">
-        <v>0.3305324521949548</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0.4367868548032215</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0.539717045707322</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0.6385396640035272</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0.7325026098958751</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0.8208907686297465</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0.9030314529469475</v>
-      </c>
-      <c r="J41" t="n">
-        <v>0.9782995226419229</v>
-      </c>
-      <c r="K41" t="n">
-        <v>1.046122142256191</v>
-      </c>
-      <c r="L41" t="n">
-        <v>1.105983140702069</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>68541.51020408163</v>
-      </c>
-      <c r="B42" t="n">
-        <v>0.223945817985936</v>
-      </c>
-      <c r="C42" t="n">
-        <v>0.33378664576024</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0.4410871556144212</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0.5450307258786704</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0.6448262832204326</v>
-      </c>
-      <c r="G42" t="n">
-        <v>0.7397143231901322</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0.8289726905086345</v>
-      </c>
-      <c r="I42" t="n">
-        <v>0.9119220751049704</v>
-      </c>
-      <c r="J42" t="n">
-        <v>0.9879311820761535</v>
-      </c>
-      <c r="K42" t="n">
-        <v>1.05642153622258</v>
-      </c>
-      <c r="L42" t="n">
-        <v>1.116871884593588</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>70199.89795918367</v>
-      </c>
-      <c r="B43" t="n">
-        <v>0.2260976671708832</v>
-      </c>
-      <c r="C43" t="n">
-        <v>0.336993932808889</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0.4453254711357191</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0.550267813732335</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0.6510222860056576</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0.7468220855844733</v>
-      </c>
-      <c r="H43" t="n">
-        <v>0.8369381181484865</v>
-      </c>
-      <c r="I43" t="n">
-        <v>0.920684546276337</v>
-      </c>
-      <c r="J43" t="n">
-        <v>0.9974240090824962</v>
-      </c>
-      <c r="K43" t="n">
-        <v>1.066572472918454</v>
-      </c>
-      <c r="L43" t="n">
-        <v>1.127603676221436</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>71858.28571428571</v>
-      </c>
-      <c r="B44" t="n">
-        <v>0.2282192269630816</v>
-      </c>
-      <c r="C44" t="n">
-        <v>0.3401560741392627</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0.449504128199391</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0.5554311844259084</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0.6571310739604258</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0.7538297992355135</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0.8447914245635412</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0.9293236770516317</v>
-      </c>
-      <c r="J44" t="n">
-        <v>1.006783215216381</v>
-      </c>
-      <c r="K44" t="n">
-        <v>1.076580525201007</v>
-      </c>
-      <c r="L44" t="n">
-        <v>1.138184407331759</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>73516.67346938775</v>
-      </c>
-      <c r="B45" t="n">
-        <v>0.230311608310696</v>
-      </c>
-      <c r="C45" t="n">
-        <v>0.3432747255968013</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0.4536253149461686</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0.5605235417423415</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0.663155845932487</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0.7607411337106386</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0.8525367221131965</v>
-      </c>
-      <c r="I45" t="n">
-        <v>0.9378439912847258</v>
-      </c>
-      <c r="J45" t="n">
-        <v>1.016013701396894</v>
-      </c>
-      <c r="K45" t="n">
-        <v>1.086450933755585</v>
-      </c>
-      <c r="L45" t="n">
-        <v>1.148619618491386</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>75175.06122448979</v>
-      </c>
-      <c r="B46" t="n">
-        <v>0.2323758574278642</v>
-      </c>
-      <c r="C46" t="n">
-        <v>0.3463514465422061</v>
-      </c>
-      <c r="D46" t="n">
-        <v>0.4576910920156405</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0.5655474319173984</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0.6690996143753889</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.7675595447545895</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0.860177883533083</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0.946249749228283</v>
-      </c>
-      <c r="J46" t="n">
-        <v>1.025120082970636</v>
-      </c>
-      <c r="K46" t="n">
-        <v>1.096188633897152</v>
-      </c>
-      <c r="L46" t="n">
-        <v>1.158914527422917</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>76833.44897959183</v>
-      </c>
-      <c r="B47" t="n">
-        <v>0.2344129609032669</v>
-      </c>
-      <c r="C47" t="n">
-        <v>0.3493877074656581</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0.4617034026081698</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0.5705052560726966</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0.6749652200580181</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0.7742882911635554</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0.867718560845285</v>
-      </c>
-      <c r="I47" t="n">
-        <v>0.9545449683361898</v>
-      </c>
-      <c r="J47" t="n">
-        <v>1.034106712248046</v>
-      </c>
-      <c r="K47" t="n">
-        <v>1.10579827966899</v>
-      </c>
-      <c r="L47" t="n">
-        <v>1.169074054482395</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>78491.83673469388</v>
-      </c>
-      <c r="B48" t="n">
-        <v>0.2364238503045851</v>
-      </c>
-      <c r="C48" t="n">
-        <v>0.3523848968496677</v>
-      </c>
-      <c r="D48" t="n">
-        <v>0.4656640815539062</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0.5753992814218594</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0.6807553453226067</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0.7809304499941332</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0.8751622024025061</v>
-      </c>
-      <c r="I48" t="n">
-        <v>0.9627334420132102</v>
-      </c>
-      <c r="J48" t="n">
-        <v>1.042977698815848</v>
-      </c>
-      <c r="K48" t="n">
-        <v>1.115284265563344</v>
-      </c>
-      <c r="L48" t="n">
-        <v>1.179102845622851</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>80150.22448979592</v>
-      </c>
-      <c r="B49" t="n">
-        <v>0.2384094063381365</v>
-      </c>
-      <c r="C49" t="n">
-        <v>0.3553443273689273</v>
-      </c>
-      <c r="D49" t="n">
-        <v>0.4695748635056695</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0.5802316513940786</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0.6864725260619287</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0.7874889303030034</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0.8825120682856554</v>
-      </c>
-      <c r="I49" t="n">
-        <v>0.9708187565532975</v>
-      </c>
-      <c r="J49" t="n">
-        <v>1.051736927887177</v>
-      </c>
-      <c r="K49" t="n">
-        <v>1.124650746143714</v>
-      </c>
-      <c r="L49" t="n">
-        <v>1.189005293139411</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>81808.61224489796</v>
-      </c>
-      <c r="B50" t="n">
-        <v>0.2403704626149324</v>
-      </c>
-      <c r="C50" t="n">
-        <v>0.3582672415035413</v>
-      </c>
-      <c r="D50" t="n">
-        <v>0.4734373903566331</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0.5850043947997988</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0.6921191625632265</v>
-      </c>
-      <c r="G50" t="n">
-        <v>0.7939664855865717</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0.8897712442445314</v>
-      </c>
-      <c r="I50" t="n">
-        <v>0.9788043064752239</v>
-      </c>
-      <c r="J50" t="n">
-        <v>1.060388076915441</v>
-      </c>
-      <c r="K50" t="n">
-        <v>1.133901653810504</v>
-      </c>
-      <c r="L50" t="n">
-        <v>1.198785554451532</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>83467</v>
-      </c>
-      <c r="B51" t="n">
-        <v>0.2423078090675773</v>
-      </c>
-      <c r="C51" t="n">
-        <v>0.361154816631845</v>
-      </c>
-      <c r="D51" t="n">
-        <v>0.4772532179703038</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0.5897194341466367</v>
-      </c>
-      <c r="F51" t="n">
-        <v>0.6976975293467836</v>
-      </c>
-      <c r="G51" t="n">
-        <v>0.8003657250673152</v>
-      </c>
-      <c r="H51" t="n">
-        <v>0.8969426543460464</v>
-      </c>
-      <c r="I51" t="n">
-        <v>0.986693308436422</v>
-      </c>
-      <c r="J51" t="n">
-        <v>1.068934630667888</v>
-      </c>
-      <c r="K51" t="n">
-        <v>1.143040714919594</v>
-      </c>
-      <c r="L51" t="n">
-        <v>1.208447569143907</v>
+        <v>8.4</v>
+      </c>
+      <c r="M12" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="N12" t="n">
+        <v>9.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>